<commit_message>
changes in find window and find pane
</commit_message>
<xml_diff>
--- a/ExcelHolder/main.xlsx
+++ b/ExcelHolder/main.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2225FAD7-3A58-4F5F-A1AE-6BA4DE8E1791}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20610" windowHeight="7665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20610" windowHeight="7665" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="workbooks (2)" sheetId="5" r:id="rId1"/>
@@ -13,7 +12,7 @@
     <sheet name="Apps" sheetId="4" r:id="rId3"/>
     <sheet name="settings" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -103,9 +102,6 @@
     <t>C:\\Program Files (x86)\\Microsoft\\Edge\\Application\\msedge.exe</t>
   </si>
   <si>
-    <t>C:\\WINDOWS\\SYSTEM32\\notepad.exe</t>
-  </si>
-  <si>
     <t>C:\\PROGRAM FILES\\MICROSOFT OFFICE\\ROOT\\OFFICE16\\winword.exe</t>
   </si>
   <si>
@@ -268,13 +264,16 @@
     <t>D:\Selenium Workspace\Epi\Automation-Framework\Finalized\CaptureSettings.xls</t>
   </si>
   <si>
-    <t>D:\Selenium Workspace\Epi\Automation-Framework\NewTestcases\2_Capture Test.xls</t>
+    <t>C:\Users\HP\git\Desktop-Framework\Finalized\2_Capture Test.xls</t>
+  </si>
+  <si>
+    <t>C:\WINDOWS\system32\\notepad.exe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -697,7 +696,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9818FA36-8E51-447B-BD69-A1B522E77535}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -716,57 +715,57 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -775,10 +774,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -794,7 +793,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -803,11 +802,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996744EF-ED44-4E17-AE14-3AC7C6B98AFA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,15 +825,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>25</v>
@@ -842,154 +841,154 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -999,7 +998,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F4E7148-1519-4393-A8E8-1ECAE413BE26}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -1057,7 +1056,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1089,7 +1088,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1097,7 +1096,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1105,7 +1104,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1126,7 +1125,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="11">
         <v>100</v>
@@ -1134,7 +1133,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{AD8227C9-5B93-4A6A-9D6D-5C57823DE336}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>